<commit_message>
missed some parts for the BOM
</commit_message>
<xml_diff>
--- a/Kick Drum/BOM.xlsx
+++ b/Kick Drum/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3F3533-BBAE-4E5F-8483-F0A9E0360EF2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566D4D6A-2087-4C76-ADD1-D64D46E3E51C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,7 +617,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +688,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f>(F2-G2)*E2</f>
+        <f t="shared" ref="H2:H8" si="0">(F2-G2)*E2</f>
         <v>1.8900000000000001</v>
       </c>
       <c r="I2" t="s">
@@ -696,7 +696,7 @@
       </c>
       <c r="K2">
         <f>SUM(H:H)</f>
-        <v>27.509999999999991</v>
+        <v>27.809999999999995</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f>(F3-G3)*E3</f>
+        <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
@@ -749,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <f>(F4-G4)*E4</f>
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="I4" t="s">
@@ -779,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="H5">
-        <f>(F5-G5)*E5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I5" t="s">
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <f>(F6-G6)*E6</f>
+        <f t="shared" si="0"/>
         <v>10.78</v>
       </c>
       <c r="I6" t="s">
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <f>(F7-G7)*E7</f>
+        <f t="shared" si="0"/>
         <v>2.48</v>
       </c>
       <c r="I7" t="s">
@@ -869,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <f>(F8-G8)*E8</f>
+        <f t="shared" si="0"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="I8" t="s">
@@ -878,13 +878,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9">
-        <f t="shared" ref="H9:H31" si="0">(F9-G9)*E9</f>
+        <f t="shared" ref="H9:H31" si="1">(F9-G9)*E9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -893,7 +893,7 @@
         <v>37</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -905,14 +905,14 @@
         <v>0.15</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
+        <f t="shared" si="1"/>
+        <v>0.3</v>
       </c>
       <c r="I12" t="s">
         <v>81</v>
@@ -932,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
     </row>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
     </row>
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
     </row>
@@ -980,14 +980,14 @@
         <v>0.15</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
+        <f t="shared" si="1"/>
+        <v>0.3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
     </row>
@@ -1022,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
     </row>
@@ -1076,13 +1076,13 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
         <v>45</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I23" t="s">
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.7399999999999993</v>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
     </row>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.33</v>
       </c>
     </row>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82</v>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37</v>
       </c>
     </row>

</xml_diff>